<commit_message>
Update to Forms for My NS Account
</commit_message>
<xml_diff>
--- a/Forms/MyNSAccount - Login Support Help Desk Forms_APPNAME.xlsx
+++ b/Forms/MyNSAccount - Login Support Help Desk Forms_APPNAME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dohanlon/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhall\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7EEC71-A3D1-7C4F-8B65-C643D311EAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B004DB-1312-461E-A066-F546FA322CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helpdesk Form" sheetId="7" r:id="rId1"/>
@@ -157,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -584,11 +584,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -835,6 +844,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1766,7 +1781,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>NSiD Login</a:t>
+            <a:t>My NS Account</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Login</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -1790,7 +1829,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> Desk (dependent on their communication method detailed below).This Shared Secret will be required for authentication when communicating with the L2 Login</a:t>
+            <a:t> Desk (dependant on their communication method detailed below).This Shared Secret will be required for authentication when communicating with the L2 Login</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -2159,6 +2198,17 @@
             <a:t>  </a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -2466,22 +2516,22 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.08203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18.5">
       <c r="A1" s="10"/>
       <c r="B1" s="42"/>
       <c r="C1" s="43"/>
@@ -2497,7 +2547,7 @@
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="28.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="41" t="s">
         <v>0</v>
@@ -2515,7 +2565,7 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="41"/>
       <c r="C3" s="39"/>
@@ -2531,7 +2581,7 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="41"/>
       <c r="C4" s="39"/>
@@ -2547,7 +2597,7 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="26.25" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="38" t="s">
         <v>1</v>
@@ -2565,7 +2615,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="18.75" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="49" t="s">
         <v>2</v>
@@ -2587,7 +2637,7 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="35" t="s">
         <v>5</v>
@@ -2605,7 +2655,7 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="35" t="s">
         <v>6</v>
@@ -2623,7 +2673,7 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="18.5">
       <c r="A9" s="10"/>
       <c r="B9" s="46" t="s">
         <v>7</v>
@@ -2641,7 +2691,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="18.5">
       <c r="A10" s="10"/>
       <c r="B10" s="1"/>
       <c r="C10" s="12"/>
@@ -2665,7 +2715,7 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18.5">
       <c r="A11" s="10"/>
       <c r="B11" s="35" t="s">
         <v>10</v>
@@ -2683,7 +2733,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="18.5">
       <c r="A12" s="10"/>
       <c r="B12" s="35" t="s">
         <v>11</v>
@@ -2701,7 +2751,7 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="18.5">
       <c r="A13" s="10"/>
       <c r="B13" s="55" t="s">
         <v>12</v>
@@ -2719,7 +2769,7 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="18.5">
       <c r="A14" s="10"/>
       <c r="B14" s="46" t="s">
         <v>13</v>
@@ -2737,7 +2787,7 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="18.5">
       <c r="A15" s="10"/>
       <c r="B15" s="1"/>
       <c r="C15" s="12"/>
@@ -2761,7 +2811,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
     </row>
-    <row r="16" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="18.5">
       <c r="A16" s="10"/>
       <c r="B16" s="53" t="s">
         <v>14</v>
@@ -2779,7 +2829,7 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
     </row>
-    <row r="17" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="18.5">
       <c r="A17" s="10"/>
       <c r="B17" s="57" t="s">
         <v>11</v>
@@ -2797,7 +2847,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="5.15" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="61"/>
       <c r="C18" s="61"/>
@@ -2813,7 +2863,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="19" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="62" t="s">
         <v>15</v>
@@ -2831,7 +2881,7 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
     </row>
-    <row r="20" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="18.5">
       <c r="A20" s="10"/>
       <c r="B20" s="57" t="s">
         <v>11</v>
@@ -2849,7 +2899,7 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
     </row>
-    <row r="21" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="5.15" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="68"/>
       <c r="C21" s="68"/>
@@ -2865,7 +2915,7 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
     </row>
-    <row r="22" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="19" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="62" t="s">
         <v>16</v>
@@ -2883,7 +2933,7 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
     </row>
-    <row r="23" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="18.5">
       <c r="A23" s="10"/>
       <c r="B23" s="66" t="s">
         <v>11</v>
@@ -2901,12 +2951,12 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
     </row>
-    <row r="24" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="5.15" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="68"/>
       <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
       <c r="F24" s="68"/>
       <c r="G24" s="68"/>
       <c r="H24" s="33"/>
@@ -2917,14 +2967,14 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
     </row>
-    <row r="25" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="19" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="62" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="63"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
       <c r="F25" s="20"/>
       <c r="G25" s="13"/>
       <c r="H25" s="32"/>
@@ -2935,12 +2985,14 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
     </row>
-    <row r="26" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="18.5">
       <c r="A26" s="10"/>
       <c r="B26" s="57" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="58"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="20"/>
       <c r="G26" s="13"/>
       <c r="H26" s="31"/>
@@ -2951,7 +3003,7 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
     </row>
-    <row r="27" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="5.15" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="68"/>
       <c r="C27" s="68"/>
@@ -2967,7 +3019,7 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
     </row>
-    <row r="28" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="19" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="71" t="s">
         <v>18</v>
@@ -2985,7 +3037,7 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
     </row>
-    <row r="29" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="5.15" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="68"/>
       <c r="C29" s="68"/>
@@ -3001,7 +3053,7 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
     </row>
-    <row r="30" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="19" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="71" t="s">
         <v>19</v>
@@ -3019,7 +3071,7 @@
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
     </row>
-    <row r="31" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="18.5">
       <c r="A31" s="10"/>
       <c r="B31" s="53" t="s">
         <v>20</v>
@@ -3037,7 +3089,7 @@
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
     </row>
-    <row r="32" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="18.5">
       <c r="A32" s="10"/>
       <c r="B32" s="46" t="s">
         <v>21</v>
@@ -3055,7 +3107,7 @@
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
     </row>
-    <row r="33" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="17.5">
       <c r="A33" s="10"/>
       <c r="B33" s="75" t="s">
         <v>22</v>
@@ -3073,7 +3125,7 @@
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
     </row>
-    <row r="34" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="18.5">
       <c r="A34" s="10"/>
       <c r="B34" s="2"/>
       <c r="C34" s="21" t="s">
@@ -3101,7 +3153,7 @@
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
     </row>
-    <row r="35" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="18.5">
       <c r="A35" s="10"/>
       <c r="B35" s="7"/>
       <c r="C35" s="19"/>
@@ -3117,7 +3169,7 @@
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
     </row>
-    <row r="36" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="18.5">
       <c r="A36" s="10"/>
       <c r="B36" s="7"/>
       <c r="C36" s="19"/>
@@ -3133,7 +3185,7 @@
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
     </row>
-    <row r="37" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="18.5">
       <c r="A37" s="10"/>
       <c r="B37" s="7"/>
       <c r="C37" s="19"/>
@@ -3149,7 +3201,7 @@
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
     </row>
-    <row r="38" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="18.5">
       <c r="A38" s="10"/>
       <c r="B38" s="7"/>
       <c r="C38" s="19"/>
@@ -3165,7 +3217,7 @@
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
     </row>
-    <row r="39" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="18.5">
       <c r="A39" s="10"/>
       <c r="B39" s="7"/>
       <c r="C39" s="19"/>
@@ -3181,7 +3233,7 @@
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
     </row>
-    <row r="40" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="18.5">
       <c r="A40" s="10"/>
       <c r="B40" s="7"/>
       <c r="C40" s="19"/>
@@ -3197,7 +3249,7 @@
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
     </row>
-    <row r="41" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="18.5">
       <c r="A41" s="10"/>
       <c r="B41" s="7"/>
       <c r="C41" s="19"/>
@@ -3213,7 +3265,7 @@
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
     </row>
-    <row r="42" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="17.5">
       <c r="A42" s="10"/>
       <c r="B42" s="75" t="s">
         <v>26</v>
@@ -3231,7 +3283,7 @@
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
     </row>
-    <row r="43" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="18.5">
       <c r="A43" s="10"/>
       <c r="B43" s="2"/>
       <c r="C43" s="21" t="s">
@@ -3259,7 +3311,7 @@
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
     </row>
-    <row r="44" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="18.5">
       <c r="A44" s="10"/>
       <c r="B44" s="7"/>
       <c r="C44" s="19"/>
@@ -3275,7 +3327,7 @@
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
     </row>
-    <row r="45" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="18.5">
       <c r="A45" s="10"/>
       <c r="B45" s="7"/>
       <c r="C45" s="19"/>
@@ -3291,7 +3343,7 @@
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
     </row>
-    <row r="46" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="18.5">
       <c r="A46" s="10"/>
       <c r="B46" s="7"/>
       <c r="C46" s="19"/>
@@ -3307,7 +3359,7 @@
       <c r="M46" s="10"/>
       <c r="N46" s="10"/>
     </row>
-    <row r="47" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="18.5">
       <c r="A47" s="10"/>
       <c r="B47" s="7"/>
       <c r="C47" s="19"/>
@@ -3323,7 +3375,7 @@
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
     </row>
-    <row r="48" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="18.5">
       <c r="A48" s="10"/>
       <c r="B48" s="7"/>
       <c r="C48" s="19"/>
@@ -3339,7 +3391,7 @@
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
     </row>
-    <row r="49" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="18.5">
       <c r="A49" s="10"/>
       <c r="B49" s="7"/>
       <c r="C49" s="19"/>
@@ -3355,7 +3407,7 @@
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
     </row>
-    <row r="50" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="18.5">
       <c r="A50" s="10"/>
       <c r="B50" s="46" t="s">
         <v>27</v>
@@ -3373,7 +3425,7 @@
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
     </row>
-    <row r="51" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="17.5">
       <c r="A51" s="10"/>
       <c r="B51" s="75" t="s">
         <v>22</v>
@@ -3391,7 +3443,7 @@
       <c r="M51" s="10"/>
       <c r="N51" s="10"/>
     </row>
-    <row r="52" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="18.5">
       <c r="A52" s="10"/>
       <c r="B52" s="2"/>
       <c r="C52" s="21" t="s">
@@ -3418,7 +3470,7 @@
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="18.5">
       <c r="A53" s="10"/>
       <c r="B53" s="7"/>
       <c r="C53" s="19"/>
@@ -3434,7 +3486,7 @@
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
     </row>
-    <row r="54" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="18.5">
       <c r="A54" s="10"/>
       <c r="B54" s="7"/>
       <c r="C54" s="19"/>
@@ -3450,7 +3502,7 @@
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
     </row>
-    <row r="55" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="18.5">
       <c r="A55" s="10"/>
       <c r="B55" s="7"/>
       <c r="C55" s="19"/>
@@ -3466,7 +3518,7 @@
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
     </row>
-    <row r="56" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="18.5">
       <c r="A56" s="10"/>
       <c r="B56" s="7"/>
       <c r="C56" s="19"/>
@@ -3482,7 +3534,7 @@
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
     </row>
-    <row r="57" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="18.5">
       <c r="A57" s="10"/>
       <c r="B57" s="7"/>
       <c r="C57" s="19"/>
@@ -3498,7 +3550,7 @@
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
     </row>
-    <row r="58" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="18.5">
       <c r="A58" s="10"/>
       <c r="B58" s="7"/>
       <c r="C58" s="19"/>
@@ -3514,7 +3566,7 @@
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
     </row>
-    <row r="59" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="17.5">
       <c r="A59" s="10"/>
       <c r="B59" s="75" t="s">
         <v>26</v>
@@ -3532,7 +3584,7 @@
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
     </row>
-    <row r="60" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="18.5">
       <c r="A60" s="10"/>
       <c r="B60" s="2"/>
       <c r="C60" s="21" t="s">
@@ -3560,7 +3612,7 @@
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
     </row>
-    <row r="61" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="18.5">
       <c r="A61" s="10"/>
       <c r="B61" s="7"/>
       <c r="C61" s="19"/>
@@ -3576,7 +3628,7 @@
       <c r="M61" s="10"/>
       <c r="N61" s="10"/>
     </row>
-    <row r="62" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="18.5">
       <c r="A62" s="10"/>
       <c r="B62" s="7"/>
       <c r="C62" s="19"/>
@@ -3592,7 +3644,7 @@
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
     </row>
-    <row r="63" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="18.5">
       <c r="A63" s="10"/>
       <c r="B63" s="7"/>
       <c r="C63" s="19"/>
@@ -3608,7 +3660,7 @@
       <c r="M63" s="10"/>
       <c r="N63" s="10"/>
     </row>
-    <row r="64" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="18.5">
       <c r="A64" s="10"/>
       <c r="B64" s="7"/>
       <c r="C64" s="19"/>
@@ -3624,7 +3676,7 @@
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
     </row>
-    <row r="65" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="18.5">
       <c r="A65" s="10"/>
       <c r="B65" s="7"/>
       <c r="C65" s="19"/>
@@ -3640,7 +3692,7 @@
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
     </row>
-    <row r="66" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="18.5">
       <c r="A66" s="10"/>
       <c r="B66" s="7"/>
       <c r="C66" s="19"/>
@@ -3656,7 +3708,7 @@
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
     </row>
-    <row r="67" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="18.5">
       <c r="A67" s="10"/>
       <c r="B67" s="46" t="s">
         <v>28</v>
@@ -3674,7 +3726,7 @@
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
     </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="15.75" customHeight="1">
       <c r="A68" s="10"/>
       <c r="B68" s="78"/>
       <c r="C68" s="79"/>
@@ -3690,7 +3742,7 @@
       <c r="M68" s="10"/>
       <c r="N68" s="10"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="15.75" customHeight="1">
       <c r="A69" s="10"/>
       <c r="B69" s="81"/>
       <c r="C69" s="82"/>
@@ -3706,7 +3758,7 @@
       <c r="M69" s="10"/>
       <c r="N69" s="10"/>
     </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="15.75" customHeight="1">
       <c r="A70" s="10"/>
       <c r="B70" s="81"/>
       <c r="C70" s="82"/>
@@ -3722,7 +3774,7 @@
       <c r="M70" s="10"/>
       <c r="N70" s="10"/>
     </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="15.75" customHeight="1">
       <c r="A71" s="10"/>
       <c r="B71" s="84"/>
       <c r="C71" s="85"/>
@@ -3738,7 +3790,7 @@
       <c r="M71" s="10"/>
       <c r="N71" s="10"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -3753,7 +3805,7 @@
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -3768,7 +3820,7 @@
       <c r="L73" s="10"/>
       <c r="M73" s="10"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -3783,7 +3835,7 @@
       <c r="L74" s="10"/>
       <c r="M74" s="10"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -3798,7 +3850,7 @@
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -3813,7 +3865,7 @@
       <c r="L76" s="10"/>
       <c r="M76" s="10"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -3828,7 +3880,7 @@
       <c r="L77" s="10"/>
       <c r="M77" s="10"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -3843,7 +3895,7 @@
       <c r="L78" s="10"/>
       <c r="M78" s="10"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -3858,7 +3910,7 @@
       <c r="L79" s="10"/>
       <c r="M79" s="10"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -3873,7 +3925,7 @@
       <c r="L80" s="10"/>
       <c r="M80" s="10"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
@@ -3888,7 +3940,7 @@
       <c r="L81" s="10"/>
       <c r="M81" s="10"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -3903,7 +3955,7 @@
       <c r="L82" s="10"/>
       <c r="M82" s="10"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -3918,7 +3970,7 @@
       <c r="L83" s="10"/>
       <c r="M83" s="10"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -3933,7 +3985,7 @@
       <c r="L84" s="10"/>
       <c r="M84" s="10"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -3948,7 +4000,7 @@
       <c r="L85" s="10"/>
       <c r="M85" s="10"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -3963,7 +4015,7 @@
       <c r="L86" s="10"/>
       <c r="M86" s="10"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
@@ -3978,7 +4030,7 @@
       <c r="L87" s="10"/>
       <c r="M87" s="10"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -3993,7 +4045,7 @@
       <c r="L88" s="10"/>
       <c r="M88" s="10"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -4008,7 +4060,7 @@
       <c r="L89" s="10"/>
       <c r="M89" s="10"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -4023,7 +4075,7 @@
       <c r="L90" s="10"/>
       <c r="M90" s="10"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -4038,7 +4090,7 @@
       <c r="L91" s="10"/>
       <c r="M91" s="10"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -4053,7 +4105,7 @@
       <c r="L92" s="10"/>
       <c r="M92" s="10"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
@@ -4068,7 +4120,7 @@
       <c r="L93" s="10"/>
       <c r="M93" s="10"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -4083,7 +4135,7 @@
       <c r="L94" s="10"/>
       <c r="M94" s="10"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
@@ -4098,7 +4150,7 @@
       <c r="L95" s="10"/>
       <c r="M95" s="10"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -4113,7 +4165,7 @@
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13">
       <c r="A97" s="10"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -4128,7 +4180,7 @@
       <c r="L97" s="10"/>
       <c r="M97" s="10"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -4143,7 +4195,7 @@
       <c r="L98" s="10"/>
       <c r="M98" s="10"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -4158,7 +4210,7 @@
       <c r="L99" s="10"/>
       <c r="M99" s="10"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13">
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
@@ -4173,7 +4225,7 @@
       <c r="L100" s="10"/>
       <c r="M100" s="10"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13">
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -4188,7 +4240,7 @@
       <c r="L101" s="10"/>
       <c r="M101" s="10"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13">
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
@@ -4203,7 +4255,7 @@
       <c r="M102" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="53">
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B51:H51"/>
     <mergeCell ref="B59:H59"/>
@@ -4218,7 +4270,7 @@
     <mergeCell ref="B33:H33"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:E28"/>
@@ -4231,6 +4283,7 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:G18"/>
@@ -4444,7 +4497,7 @@
       <formula>$G34="REMOVE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:E25">
+  <conditionalFormatting sqref="D26:E26">
     <cfRule type="expression" dxfId="2" priority="259">
       <formula>$G26="UPDATE"</formula>
     </cfRule>
@@ -4466,7 +4519,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Provides French support for international calls." sqref="B23:E23" xr:uid="{E5C98B2D-27B7-4469-8D5D-C065C4DA6CA5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Identified Authorized Representatives will receive notifications for incidents in the TEST environment." sqref="C53:C58" xr:uid="{5FA3A8E3-4BD6-4948-8012-D9C811402F04}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Identified Authorized Representatives will receive notifications for incidents in the PROD environment." sqref="C61:C66" xr:uid="{88BEB61B-DC6E-43B1-BAC4-78D64035A5DE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Provides French Teletype support to callers." sqref="D25:E25 B26:C26" xr:uid="{2E019E40-F87C-4E9C-8D65-F0254E4D45EE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Provides French Teletype support to callers." sqref="D26:E26 B26:C26" xr:uid="{2E019E40-F87C-4E9C-8D65-F0254E4D45EE}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Provides Teletype support for calls related to your organization but not specific to any online application." sqref="B13:C13 D13:E13" xr:uid="{854EA2FD-DF28-4A9E-9F68-D99E18319445}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Provides French support for calls related to your organization but not specific to any online application." sqref="B12:E12" xr:uid="{F7A4DE1C-4D0D-49FB-AE94-F808866BA4D8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Provides English support for calls related to your organization but not specific to any online application." sqref="B11:C11 D11:E11" xr:uid="{2EC92221-B9D7-4B0B-8F75-9ACF13DC58B8}"/>
@@ -4508,11 +4561,11 @@
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.33203125" bestFit="1" customWidth="1"/>
@@ -4526,28 +4579,28 @@
     <col min="15" max="15" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16384" ht="17">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16384" ht="17">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16384" ht="17">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16384" ht="17">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16384" ht="17">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -4555,18 +4608,18 @@
       <c r="E7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16384" ht="17">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16384" ht="17">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:16384" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16384" customFormat="1" ht="17">
       <c r="A10" s="4"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
@@ -20952,7 +21005,7 @@
       <c r="XFC10" s="6"/>
       <c r="XFD10" s="6"/>
     </row>
-    <row r="11" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16384" ht="17">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -20963,13 +21016,13 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16384" ht="17">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16384" ht="17">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -20978,25 +21031,25 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16384" ht="17">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16384" ht="17">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:16384" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16384" ht="17">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="17">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -21013,12 +21066,12 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="17">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="17">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -21026,7 +21079,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="17">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -21034,62 +21087,62 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="17">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="17">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="17">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="17">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="F24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="17">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="17">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="17">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="17">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="17">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="17">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
@@ -21098,19 +21151,19 @@
       <c r="F30" s="6"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="17">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="17">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="17">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -21119,79 +21172,79 @@
       <c r="F33" s="6"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="17">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="17">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="17">
       <c r="A39" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="17">
       <c r="A40" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="17">
       <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="17">
       <c r="A42" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="17">
       <c r="A43" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="17">
       <c r="A44" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="17">
       <c r="A45" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="17">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="17">
       <c r="A48" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="17">
       <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="17">
       <c r="A50" s="4" t="s">
         <v>37</v>
       </c>
@@ -21202,10 +21255,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B0A5F5B3655444BBCEB85CFA4561AA6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="697c50b32b01ba6de16719ccb77208a8">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e5f6f2d-25bb-4120-8159-3f6098a64328" xmlns:ns3="150c0b57-9b77-4f1c-a002-8cd409c927e7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b93a6c30582b9ee29ace120fb110a3fc" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B0A5F5B3655444BBCEB85CFA4561AA6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deb3aa6c615fef720b17435163ba86bb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e5f6f2d-25bb-4120-8159-3f6098a64328" xmlns:ns3="150c0b57-9b77-4f1c-a002-8cd409c927e7" xmlns:ns4="fb5252e3-2a48-4ca4-b8bb-926e687cdbbb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e27ee979364a9177e63ba0ec207a7b16" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5e5f6f2d-25bb-4120-8159-3f6098a64328"/>
     <xsd:import namespace="150c0b57-9b77-4f1c-a002-8cd409c927e7"/>
+    <xsd:import namespace="fb5252e3-2a48-4ca4-b8bb-926e687cdbbb"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -21229,6 +21283,7 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:Expiry_x0020_Date" minOccurs="0"/>
+                <xsd:element ref="ns4:Classification" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -21357,6 +21412,20 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5252e3-2a48-4ca4-b8bb-926e687cdbbb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Classification" ma:index="26" nillable="true" ma:displayName="Classification" ma:default="TLP-Green" ma:description="Used to apply a classification to non-Microsoft documents that do not have a sensitivity label." ma:format="Dropdown" ma:internalName="Classification">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="TLP-White"/>
+          <xsd:enumeration value="TLP-Green"/>
+          <xsd:enumeration value="TLP-Amber"/>
+          <xsd:enumeration value="TLP-Red"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
     <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
@@ -21475,12 +21544,13 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
     <TaxCatchAll xmlns="150c0b57-9b77-4f1c-a002-8cd409c927e7" xsi:nil="true"/>
     <Expiry_x0020_Date xmlns="5e5f6f2d-25bb-4120-8159-3f6098a64328" xsi:nil="true"/>
+    <Classification xmlns="fb5252e3-2a48-4ca4-b8bb-926e687cdbbb">TLP-Green</Classification>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8913D7FD-8AED-41F4-ACDB-83A6AE6CED9A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B469E167-C97D-452F-BAC9-FC7AE7B70884}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -21488,6 +21558,7 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="5e5f6f2d-25bb-4120-8159-3f6098a64328"/>
     <ds:schemaRef ds:uri="150c0b57-9b77-4f1c-a002-8cd409c927e7"/>
+    <ds:schemaRef ds:uri="fb5252e3-2a48-4ca4-b8bb-926e687cdbbb"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -21519,6 +21590,7 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="150c0b57-9b77-4f1c-a002-8cd409c927e7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fb5252e3-2a48-4ca4-b8bb-926e687cdbbb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>